<commit_message>
se agregaron campos nombre y marca
</commit_message>
<xml_diff>
--- a/GestionCodigos/data.xlsx
+++ b/GestionCodigos/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,16 @@
           <t>Ubicación</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Producto</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Marca</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -451,77 +461,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A2</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>734058</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>7340556</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>734053</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>A2</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>734056</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>734050</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>B1</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>734056</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
           <t>A21</t>
         </is>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>444444</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>A21</t>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Diego</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>PP</t>
         </is>
       </c>
     </row>

</xml_diff>